<commit_message>
add Download to Flash mirror
</commit_message>
<xml_diff>
--- a/位图关系表.xlsx
+++ b/位图关系表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>H = 18</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,12 +100,36 @@
     <t>对应的字节位置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Flash Data 数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xC0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H = 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>W = 8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0xFF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图像起点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +160,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,6 +268,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -235,7 +305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,6 +354,9 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -298,6 +371,70 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,37 +737,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D5:Q138"/>
+  <dimension ref="C5:AC150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F109" sqref="F109"/>
+    <sheetView tabSelected="1" topLeftCell="C124" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G154" sqref="G154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
     <col min="6" max="6" width="9" style="16"/>
     <col min="10" max="11" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="24"/>
+      <c r="N5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
     </row>
     <row r="6" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="23" t="s">
         <v>0</v>
       </c>
       <c r="E6" s="3">
@@ -671,7 +808,7 @@
       </c>
     </row>
     <row r="7" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D7" s="22"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="3">
         <v>13</v>
       </c>
@@ -710,7 +847,7 @@
       </c>
     </row>
     <row r="8" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D8" s="22"/>
+      <c r="D8" s="23"/>
       <c r="E8" s="3">
         <v>25</v>
       </c>
@@ -749,7 +886,7 @@
       </c>
     </row>
     <row r="9" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D9" s="22"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="3">
         <v>37</v>
       </c>
@@ -788,7 +925,7 @@
       </c>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D10" s="22"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="3">
         <v>49</v>
       </c>
@@ -827,7 +964,7 @@
       </c>
     </row>
     <row r="11" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D11" s="22"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="3">
         <v>61</v>
       </c>
@@ -866,7 +1003,7 @@
       </c>
     </row>
     <row r="12" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D12" s="22"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="3">
         <v>73</v>
       </c>
@@ -905,7 +1042,7 @@
       </c>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D13" s="22"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="3">
         <v>85</v>
       </c>
@@ -944,7 +1081,7 @@
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D14" s="22"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="6">
         <v>97</v>
       </c>
@@ -983,7 +1120,7 @@
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D15" s="22"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="6">
         <v>109</v>
       </c>
@@ -1022,7 +1159,7 @@
       </c>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D16" s="22"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="6">
         <v>121</v>
       </c>
@@ -1061,7 +1198,7 @@
       </c>
     </row>
     <row r="17" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D17" s="22"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="6">
         <v>133</v>
       </c>
@@ -1100,7 +1237,7 @@
       </c>
     </row>
     <row r="18" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D18" s="22"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="6">
         <v>145</v>
       </c>
@@ -1139,7 +1276,7 @@
       </c>
     </row>
     <row r="19" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D19" s="22"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="6">
         <v>157</v>
       </c>
@@ -1178,7 +1315,7 @@
       </c>
     </row>
     <row r="20" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D20" s="22"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="6">
         <v>169</v>
       </c>
@@ -1217,7 +1354,7 @@
       </c>
     </row>
     <row r="21" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D21" s="22"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="6">
         <v>181</v>
       </c>
@@ -1256,7 +1393,7 @@
       </c>
     </row>
     <row r="22" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D22" s="22"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="7">
         <v>193</v>
       </c>
@@ -1295,7 +1432,7 @@
       </c>
     </row>
     <row r="23" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D23" s="22"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="7">
         <v>205</v>
       </c>
@@ -1418,23 +1555,23 @@
       <c r="P29" s="7"/>
     </row>
     <row r="30" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-      <c r="K30" s="23"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
     </row>
     <row r="31" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="23" t="s">
         <v>0</v>
       </c>
       <c r="E31" s="5">
@@ -1478,7 +1615,7 @@
       </c>
     </row>
     <row r="32" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D32" s="22"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="5">
         <v>12</v>
       </c>
@@ -1517,7 +1654,7 @@
       </c>
     </row>
     <row r="33" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D33" s="22"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="5">
         <v>24</v>
       </c>
@@ -1556,7 +1693,7 @@
       </c>
     </row>
     <row r="34" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D34" s="22"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="5">
         <v>36</v>
       </c>
@@ -1595,7 +1732,7 @@
       </c>
     </row>
     <row r="35" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D35" s="22"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="5">
         <v>48</v>
       </c>
@@ -1634,7 +1771,7 @@
       </c>
     </row>
     <row r="36" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D36" s="22"/>
+      <c r="D36" s="23"/>
       <c r="E36" s="5">
         <v>60</v>
       </c>
@@ -1673,7 +1810,7 @@
       </c>
     </row>
     <row r="37" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D37" s="22"/>
+      <c r="D37" s="23"/>
       <c r="E37" s="5">
         <v>72</v>
       </c>
@@ -1712,7 +1849,7 @@
       </c>
     </row>
     <row r="38" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D38" s="22"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="5">
         <v>84</v>
       </c>
@@ -1754,7 +1891,7 @@
       </c>
     </row>
     <row r="39" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D39" s="22"/>
+      <c r="D39" s="23"/>
       <c r="E39" s="6">
         <v>96</v>
       </c>
@@ -1793,7 +1930,7 @@
       </c>
     </row>
     <row r="40" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D40" s="22"/>
+      <c r="D40" s="23"/>
       <c r="E40" s="6">
         <v>108</v>
       </c>
@@ -1832,7 +1969,7 @@
       </c>
     </row>
     <row r="41" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D41" s="22"/>
+      <c r="D41" s="23"/>
       <c r="E41" s="6">
         <v>120</v>
       </c>
@@ -1871,7 +2008,7 @@
       </c>
     </row>
     <row r="42" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D42" s="22"/>
+      <c r="D42" s="23"/>
       <c r="E42" s="6">
         <v>132</v>
       </c>
@@ -1910,7 +2047,7 @@
       </c>
     </row>
     <row r="43" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D43" s="22"/>
+      <c r="D43" s="23"/>
       <c r="E43" s="6">
         <v>144</v>
       </c>
@@ -1949,7 +2086,7 @@
       </c>
     </row>
     <row r="44" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D44" s="22"/>
+      <c r="D44" s="23"/>
       <c r="E44" s="6">
         <v>156</v>
       </c>
@@ -1988,7 +2125,7 @@
       </c>
     </row>
     <row r="45" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D45" s="22"/>
+      <c r="D45" s="23"/>
       <c r="E45" s="6">
         <v>168</v>
       </c>
@@ -2027,7 +2164,7 @@
       </c>
     </row>
     <row r="46" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D46" s="22"/>
+      <c r="D46" s="23"/>
       <c r="E46" s="6">
         <v>180</v>
       </c>
@@ -2066,7 +2203,7 @@
       </c>
     </row>
     <row r="47" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D47" s="22"/>
+      <c r="D47" s="23"/>
       <c r="E47" s="8">
         <v>192</v>
       </c>
@@ -2105,7 +2242,7 @@
       </c>
     </row>
     <row r="48" spans="4:17" x14ac:dyDescent="0.15">
-      <c r="D48" s="22"/>
+      <c r="D48" s="23"/>
       <c r="E48" s="8">
         <v>204</v>
       </c>
@@ -2231,16 +2368,16 @@
       <c r="D56" t="s">
         <v>6</v>
       </c>
-      <c r="E56" s="24">
+      <c r="E56" s="25">
         <v>5</v>
       </c>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="H56" s="24"/>
-      <c r="I56" s="24"/>
+      <c r="F56" s="25"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="25"/>
+      <c r="I56" s="25"/>
     </row>
     <row r="57" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D57" s="20">
+      <c r="D57" s="21">
         <v>6</v>
       </c>
       <c r="E57" s="11">
@@ -2260,7 +2397,7 @@
       </c>
     </row>
     <row r="58" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D58" s="20"/>
+      <c r="D58" s="21"/>
       <c r="E58" s="11">
         <v>5</v>
       </c>
@@ -2278,7 +2415,7 @@
       </c>
     </row>
     <row r="59" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D59" s="20"/>
+      <c r="D59" s="21"/>
       <c r="E59" s="2">
         <v>10</v>
       </c>
@@ -2296,7 +2433,7 @@
       </c>
     </row>
     <row r="60" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D60" s="20"/>
+      <c r="D60" s="21"/>
       <c r="E60" s="11">
         <v>15</v>
       </c>
@@ -2314,7 +2451,7 @@
       </c>
     </row>
     <row r="61" spans="4:16" x14ac:dyDescent="0.15">
-      <c r="D61" s="20"/>
+      <c r="D61" s="21"/>
       <c r="E61" s="11">
         <v>20</v>
       </c>
@@ -2650,14 +2787,14 @@
       <c r="E92" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H92" s="21" t="s">
+      <c r="H92" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="I92" s="21"/>
-      <c r="J92" s="21"/>
+      <c r="I92" s="22"/>
+      <c r="J92" s="22"/>
     </row>
     <row r="93" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D93" s="20" t="s">
+      <c r="D93" s="21" t="s">
         <v>19</v>
       </c>
       <c r="E93" s="13">
@@ -2680,7 +2817,7 @@
       </c>
     </row>
     <row r="94" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D94" s="20"/>
+      <c r="D94" s="21"/>
       <c r="E94" s="13">
         <v>1</v>
       </c>
@@ -2701,7 +2838,7 @@
       </c>
     </row>
     <row r="95" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D95" s="20"/>
+      <c r="D95" s="21"/>
       <c r="E95" s="13">
         <v>2</v>
       </c>
@@ -2722,7 +2859,7 @@
       </c>
     </row>
     <row r="96" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D96" s="20"/>
+      <c r="D96" s="21"/>
       <c r="E96" s="13">
         <v>3</v>
       </c>
@@ -2743,7 +2880,7 @@
       </c>
     </row>
     <row r="97" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D97" s="20"/>
+      <c r="D97" s="21"/>
       <c r="E97" s="13">
         <v>4</v>
       </c>
@@ -2764,7 +2901,7 @@
       </c>
     </row>
     <row r="98" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D98" s="20"/>
+      <c r="D98" s="21"/>
       <c r="E98" s="13">
         <v>5</v>
       </c>
@@ -2785,7 +2922,7 @@
       </c>
     </row>
     <row r="99" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D99" s="20"/>
+      <c r="D99" s="21"/>
       <c r="E99" s="13">
         <v>6</v>
       </c>
@@ -2806,7 +2943,7 @@
       </c>
     </row>
     <row r="100" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D100" s="20"/>
+      <c r="D100" s="21"/>
       <c r="E100" s="13">
         <v>7</v>
       </c>
@@ -2827,7 +2964,7 @@
       </c>
     </row>
     <row r="101" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D101" s="20"/>
+      <c r="D101" s="21"/>
       <c r="E101" s="5">
         <v>8</v>
       </c>
@@ -2848,7 +2985,7 @@
       </c>
     </row>
     <row r="102" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D102" s="20"/>
+      <c r="D102" s="21"/>
       <c r="E102" s="5">
         <v>9</v>
       </c>
@@ -2869,7 +3006,7 @@
       </c>
     </row>
     <row r="103" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D103" s="20"/>
+      <c r="D103" s="21"/>
       <c r="E103" s="5">
         <v>10</v>
       </c>
@@ -2890,7 +3027,7 @@
       </c>
     </row>
     <row r="104" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D104" s="20"/>
+      <c r="D104" s="21"/>
       <c r="E104" s="5">
         <v>11</v>
       </c>
@@ -2911,7 +3048,7 @@
       </c>
     </row>
     <row r="105" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D105" s="20"/>
+      <c r="D105" s="21"/>
       <c r="E105" s="5">
         <v>12</v>
       </c>
@@ -2932,7 +3069,7 @@
       </c>
     </row>
     <row r="106" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D106" s="20"/>
+      <c r="D106" s="21"/>
       <c r="E106" s="5">
         <v>13</v>
       </c>
@@ -2953,7 +3090,7 @@
       </c>
     </row>
     <row r="107" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D107" s="20"/>
+      <c r="D107" s="21"/>
       <c r="E107" s="5">
         <v>14</v>
       </c>
@@ -2974,7 +3111,7 @@
       </c>
     </row>
     <row r="108" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D108" s="20"/>
+      <c r="D108" s="21"/>
       <c r="E108" s="5">
         <v>15</v>
       </c>
@@ -2995,7 +3132,7 @@
       </c>
     </row>
     <row r="109" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D109" s="20"/>
+      <c r="D109" s="21"/>
       <c r="E109" s="6">
         <v>16</v>
       </c>
@@ -3016,7 +3153,7 @@
       </c>
     </row>
     <row r="110" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D110" s="20"/>
+      <c r="D110" s="21"/>
       <c r="E110" s="6">
         <v>17</v>
       </c>
@@ -3037,7 +3174,7 @@
       </c>
     </row>
     <row r="111" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D111" s="20"/>
+      <c r="D111" s="21"/>
       <c r="E111" s="6">
         <v>18</v>
       </c>
@@ -3058,7 +3195,7 @@
       </c>
     </row>
     <row r="112" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D112" s="20"/>
+      <c r="D112" s="21"/>
       <c r="E112" s="6">
         <v>19</v>
       </c>
@@ -3079,7 +3216,7 @@
       </c>
     </row>
     <row r="113" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D113" s="20"/>
+      <c r="D113" s="21"/>
       <c r="E113" s="6">
         <v>20</v>
       </c>
@@ -3100,7 +3237,7 @@
       </c>
     </row>
     <row r="114" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D114" s="20"/>
+      <c r="D114" s="21"/>
       <c r="E114" s="6">
         <v>21</v>
       </c>
@@ -3121,7 +3258,7 @@
       </c>
     </row>
     <row r="115" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D115" s="20"/>
+      <c r="D115" s="21"/>
       <c r="E115" s="6">
         <v>22</v>
       </c>
@@ -3142,7 +3279,7 @@
       </c>
     </row>
     <row r="116" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D116" s="20"/>
+      <c r="D116" s="21"/>
       <c r="E116" s="6">
         <v>23</v>
       </c>
@@ -3163,7 +3300,7 @@
       </c>
     </row>
     <row r="117" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D117" s="20"/>
+      <c r="D117" s="21"/>
       <c r="E117" s="14">
         <v>24</v>
       </c>
@@ -3181,7 +3318,7 @@
       </c>
     </row>
     <row r="118" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D118" s="20"/>
+      <c r="D118" s="21"/>
       <c r="E118" s="14">
         <v>25</v>
       </c>
@@ -3199,7 +3336,7 @@
       </c>
     </row>
     <row r="119" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D119" s="20"/>
+      <c r="D119" s="21"/>
       <c r="E119" s="14">
         <v>26</v>
       </c>
@@ -3217,7 +3354,7 @@
       </c>
     </row>
     <row r="120" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="D120" s="20"/>
+      <c r="D120" s="21"/>
       <c r="E120" s="14">
         <v>27</v>
       </c>
@@ -3301,43 +3438,913 @@
       <c r="E126" s="1"/>
     </row>
     <row r="127" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="E127" s="1"/>
-    </row>
-    <row r="128" spans="4:11" x14ac:dyDescent="0.15">
-      <c r="E128" s="1"/>
-    </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E129" s="1"/>
-    </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E130" s="1"/>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E131" s="1"/>
-    </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E132" s="1"/>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E133" s="1"/>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E134" s="1"/>
-    </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E135" s="1"/>
-    </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E136" s="1"/>
-    </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E137" s="1"/>
-    </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E138" s="1"/>
+      <c r="E127" s="20"/>
+      <c r="F127" s="20"/>
+      <c r="J127" s="20"/>
+      <c r="K127" s="20"/>
+    </row>
+    <row r="128" spans="4:11" s="30" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E128" s="26"/>
+      <c r="F128" s="26"/>
+      <c r="J128" s="26"/>
+      <c r="K128" s="26"/>
+    </row>
+    <row r="129" spans="3:28" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E129" s="28"/>
+      <c r="F129" s="28"/>
+      <c r="J129" s="28"/>
+      <c r="K129" s="28"/>
+    </row>
+    <row r="130" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="E130" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F130" s="31"/>
+      <c r="G130" s="31"/>
+      <c r="H130" s="31"/>
+      <c r="I130" s="31"/>
+      <c r="J130" s="31"/>
+      <c r="K130" s="31"/>
+      <c r="L130" s="31"/>
+    </row>
+    <row r="131" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="E131" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F131" s="25"/>
+      <c r="G131" s="25"/>
+      <c r="H131" s="25"/>
+      <c r="I131" s="25"/>
+      <c r="J131" s="25"/>
+      <c r="K131" s="25"/>
+      <c r="L131" s="25"/>
+      <c r="N131" s="36"/>
+      <c r="O131" s="36"/>
+      <c r="P131" s="36"/>
+      <c r="Q131" s="36"/>
+      <c r="R131" s="36"/>
+    </row>
+    <row r="132" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D132" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E132" s="27">
+        <v>0</v>
+      </c>
+      <c r="F132" s="27">
+        <v>8</v>
+      </c>
+      <c r="G132" s="27">
+        <v>16</v>
+      </c>
+      <c r="H132" s="27">
+        <v>24</v>
+      </c>
+      <c r="I132" s="27">
+        <v>32</v>
+      </c>
+      <c r="J132" s="27">
+        <v>40</v>
+      </c>
+      <c r="K132" s="27">
+        <v>48</v>
+      </c>
+      <c r="L132" s="27">
+        <v>56</v>
+      </c>
+      <c r="S132" s="36"/>
+      <c r="AA132" s="20"/>
+    </row>
+    <row r="133" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D133" s="29"/>
+      <c r="E133" s="27">
+        <v>1</v>
+      </c>
+      <c r="F133" s="27">
+        <v>9</v>
+      </c>
+      <c r="G133" s="27">
+        <v>17</v>
+      </c>
+      <c r="H133" s="27">
+        <v>25</v>
+      </c>
+      <c r="I133" s="27">
+        <v>33</v>
+      </c>
+      <c r="J133" s="27">
+        <v>41</v>
+      </c>
+      <c r="K133" s="27">
+        <v>49</v>
+      </c>
+      <c r="L133" s="27">
+        <v>57</v>
+      </c>
+      <c r="S133" s="36"/>
+      <c r="AA133" s="20"/>
+    </row>
+    <row r="134" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D134" s="29"/>
+      <c r="E134" s="27">
+        <v>2</v>
+      </c>
+      <c r="F134" s="27">
+        <v>10</v>
+      </c>
+      <c r="G134" s="8">
+        <v>18</v>
+      </c>
+      <c r="H134" s="8">
+        <v>26</v>
+      </c>
+      <c r="I134" s="8">
+        <v>34</v>
+      </c>
+      <c r="J134" s="8">
+        <v>42</v>
+      </c>
+      <c r="K134" s="27">
+        <v>50</v>
+      </c>
+      <c r="L134" s="27">
+        <v>58</v>
+      </c>
+      <c r="S134" s="36"/>
+      <c r="AA134" s="20"/>
+    </row>
+    <row r="135" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D135" s="29"/>
+      <c r="E135" s="27">
+        <v>3</v>
+      </c>
+      <c r="F135" s="27">
+        <v>11</v>
+      </c>
+      <c r="G135" s="8">
+        <v>19</v>
+      </c>
+      <c r="H135" s="8">
+        <v>27</v>
+      </c>
+      <c r="I135" s="8">
+        <v>35</v>
+      </c>
+      <c r="J135" s="8">
+        <v>43</v>
+      </c>
+      <c r="K135" s="27">
+        <v>51</v>
+      </c>
+      <c r="L135" s="27">
+        <v>59</v>
+      </c>
+      <c r="S135" s="36"/>
+      <c r="AA135" s="20"/>
+    </row>
+    <row r="136" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D136" s="29"/>
+      <c r="E136" s="27">
+        <v>4</v>
+      </c>
+      <c r="F136" s="27">
+        <v>12</v>
+      </c>
+      <c r="G136" s="8">
+        <v>20</v>
+      </c>
+      <c r="H136" s="8">
+        <v>28</v>
+      </c>
+      <c r="I136" s="8">
+        <v>36</v>
+      </c>
+      <c r="J136" s="8">
+        <v>44</v>
+      </c>
+      <c r="K136" s="27">
+        <v>52</v>
+      </c>
+      <c r="L136" s="27">
+        <v>60</v>
+      </c>
+      <c r="S136" s="36"/>
+      <c r="AA136" s="20"/>
+    </row>
+    <row r="137" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D137" s="29"/>
+      <c r="E137" s="27">
+        <v>6</v>
+      </c>
+      <c r="F137" s="27">
+        <v>13</v>
+      </c>
+      <c r="G137" s="8">
+        <v>20</v>
+      </c>
+      <c r="H137" s="8">
+        <v>27</v>
+      </c>
+      <c r="I137" s="8">
+        <v>34</v>
+      </c>
+      <c r="J137" s="8">
+        <v>41</v>
+      </c>
+      <c r="K137" s="27">
+        <v>48</v>
+      </c>
+      <c r="L137" s="27">
+        <v>55</v>
+      </c>
+      <c r="S137" s="36"/>
+    </row>
+    <row r="138" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D138" s="29"/>
+      <c r="E138" s="27">
+        <v>7</v>
+      </c>
+      <c r="F138" s="27">
+        <v>14</v>
+      </c>
+      <c r="G138" s="8">
+        <v>21</v>
+      </c>
+      <c r="H138" s="8">
+        <v>28</v>
+      </c>
+      <c r="I138" s="8">
+        <v>35</v>
+      </c>
+      <c r="J138" s="8">
+        <v>42</v>
+      </c>
+      <c r="K138" s="27">
+        <v>49</v>
+      </c>
+      <c r="L138" s="27">
+        <v>56</v>
+      </c>
+      <c r="S138" s="36"/>
+    </row>
+    <row r="139" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="D139" s="34"/>
+      <c r="E139" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="F139" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G139" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="H139" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="I139" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="J139" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="K139" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L139" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="S139" s="36"/>
+    </row>
+    <row r="143" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C143">
+        <v>8</v>
+      </c>
+      <c r="E143" s="38">
+        <v>168</v>
+      </c>
+      <c r="F143" s="39">
+        <v>169</v>
+      </c>
+      <c r="G143" s="40">
+        <v>170</v>
+      </c>
+      <c r="H143" s="38">
+        <v>171</v>
+      </c>
+      <c r="I143" s="39">
+        <v>172</v>
+      </c>
+      <c r="J143" s="40">
+        <v>173</v>
+      </c>
+      <c r="K143" s="38">
+        <v>174</v>
+      </c>
+      <c r="L143" s="39">
+        <v>175</v>
+      </c>
+      <c r="M143" s="40">
+        <v>176</v>
+      </c>
+      <c r="N143" s="38">
+        <v>177</v>
+      </c>
+      <c r="O143" s="39">
+        <v>178</v>
+      </c>
+      <c r="P143" s="40">
+        <v>179</v>
+      </c>
+      <c r="Q143" s="38">
+        <v>180</v>
+      </c>
+      <c r="R143" s="39">
+        <v>181</v>
+      </c>
+      <c r="S143" s="40">
+        <v>182</v>
+      </c>
+      <c r="T143" s="38">
+        <v>183</v>
+      </c>
+      <c r="U143" s="39">
+        <v>184</v>
+      </c>
+      <c r="V143" s="40">
+        <v>185</v>
+      </c>
+      <c r="W143" s="38">
+        <v>186</v>
+      </c>
+      <c r="X143" s="39">
+        <v>187</v>
+      </c>
+      <c r="Y143" s="40">
+        <v>188</v>
+      </c>
+      <c r="Z143" s="38">
+        <v>189</v>
+      </c>
+      <c r="AA143" s="39">
+        <v>190</v>
+      </c>
+      <c r="AB143" s="40">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="144" spans="3:28" x14ac:dyDescent="0.15">
+      <c r="C144">
+        <v>7</v>
+      </c>
+      <c r="D144" s="37"/>
+      <c r="E144" s="38">
+        <v>144</v>
+      </c>
+      <c r="F144" s="39">
+        <v>145</v>
+      </c>
+      <c r="G144" s="40">
+        <v>146</v>
+      </c>
+      <c r="H144" s="38">
+        <v>147</v>
+      </c>
+      <c r="I144" s="39">
+        <v>148</v>
+      </c>
+      <c r="J144" s="40">
+        <v>149</v>
+      </c>
+      <c r="K144" s="38">
+        <v>150</v>
+      </c>
+      <c r="L144" s="39">
+        <v>151</v>
+      </c>
+      <c r="M144" s="40">
+        <v>152</v>
+      </c>
+      <c r="N144" s="41">
+        <v>153</v>
+      </c>
+      <c r="O144" s="39">
+        <v>154</v>
+      </c>
+      <c r="P144" s="40">
+        <v>155</v>
+      </c>
+      <c r="Q144" s="38">
+        <v>156</v>
+      </c>
+      <c r="R144" s="39">
+        <v>157</v>
+      </c>
+      <c r="S144" s="40">
+        <v>158</v>
+      </c>
+      <c r="T144" s="38">
+        <v>159</v>
+      </c>
+      <c r="U144" s="39">
+        <v>160</v>
+      </c>
+      <c r="V144" s="40">
+        <v>161</v>
+      </c>
+      <c r="W144" s="38">
+        <v>162</v>
+      </c>
+      <c r="X144" s="39">
+        <v>163</v>
+      </c>
+      <c r="Y144" s="40">
+        <v>164</v>
+      </c>
+      <c r="Z144" s="38">
+        <v>165</v>
+      </c>
+      <c r="AA144" s="39">
+        <v>166</v>
+      </c>
+      <c r="AB144" s="40">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="145" spans="3:29" x14ac:dyDescent="0.15">
+      <c r="C145">
+        <v>6</v>
+      </c>
+      <c r="E145" s="38">
+        <v>120</v>
+      </c>
+      <c r="F145" s="39">
+        <v>121</v>
+      </c>
+      <c r="G145" s="40">
+        <v>122</v>
+      </c>
+      <c r="H145" s="38">
+        <v>123</v>
+      </c>
+      <c r="I145" s="39">
+        <v>124</v>
+      </c>
+      <c r="J145" s="40">
+        <v>125</v>
+      </c>
+      <c r="K145" s="42">
+        <v>126</v>
+      </c>
+      <c r="L145" s="43">
+        <v>127</v>
+      </c>
+      <c r="M145" s="44">
+        <v>128</v>
+      </c>
+      <c r="N145" s="42">
+        <v>129</v>
+      </c>
+      <c r="O145" s="43">
+        <v>130</v>
+      </c>
+      <c r="P145" s="44">
+        <v>131</v>
+      </c>
+      <c r="Q145" s="42">
+        <v>132</v>
+      </c>
+      <c r="R145" s="43">
+        <v>133</v>
+      </c>
+      <c r="S145" s="44">
+        <v>134</v>
+      </c>
+      <c r="T145" s="42">
+        <v>135</v>
+      </c>
+      <c r="U145" s="43">
+        <v>136</v>
+      </c>
+      <c r="V145" s="40">
+        <v>137</v>
+      </c>
+      <c r="W145" s="38">
+        <v>138</v>
+      </c>
+      <c r="X145" s="39">
+        <v>139</v>
+      </c>
+      <c r="Y145" s="40">
+        <v>140</v>
+      </c>
+      <c r="Z145" s="38">
+        <v>141</v>
+      </c>
+      <c r="AA145" s="39">
+        <v>142</v>
+      </c>
+      <c r="AB145" s="40">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="146" spans="3:29" x14ac:dyDescent="0.15">
+      <c r="C146">
+        <v>5</v>
+      </c>
+      <c r="E146" s="38">
+        <v>96</v>
+      </c>
+      <c r="F146" s="39">
+        <v>97</v>
+      </c>
+      <c r="G146" s="40">
+        <v>98</v>
+      </c>
+      <c r="H146" s="38">
+        <v>99</v>
+      </c>
+      <c r="I146" s="39">
+        <v>100</v>
+      </c>
+      <c r="J146" s="40">
+        <v>101</v>
+      </c>
+      <c r="K146" s="46">
+        <v>102</v>
+      </c>
+      <c r="L146" s="47">
+        <v>103</v>
+      </c>
+      <c r="M146" s="48">
+        <v>104</v>
+      </c>
+      <c r="N146" s="49">
+        <v>105</v>
+      </c>
+      <c r="O146" s="47">
+        <v>106</v>
+      </c>
+      <c r="P146" s="48">
+        <v>107</v>
+      </c>
+      <c r="Q146" s="46">
+        <v>108</v>
+      </c>
+      <c r="R146" s="47">
+        <v>109</v>
+      </c>
+      <c r="S146" s="48">
+        <v>110</v>
+      </c>
+      <c r="T146" s="46">
+        <v>111</v>
+      </c>
+      <c r="U146" s="47">
+        <v>112</v>
+      </c>
+      <c r="V146" s="40">
+        <v>113</v>
+      </c>
+      <c r="W146" s="38">
+        <v>114</v>
+      </c>
+      <c r="X146" s="39">
+        <v>115</v>
+      </c>
+      <c r="Y146" s="40">
+        <v>116</v>
+      </c>
+      <c r="Z146" s="38">
+        <v>117</v>
+      </c>
+      <c r="AA146" s="39">
+        <v>118</v>
+      </c>
+      <c r="AB146" s="40">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="147" spans="3:29" x14ac:dyDescent="0.15">
+      <c r="C147">
+        <v>4</v>
+      </c>
+      <c r="E147" s="38">
+        <v>72</v>
+      </c>
+      <c r="F147" s="39">
+        <v>73</v>
+      </c>
+      <c r="G147" s="40">
+        <v>74</v>
+      </c>
+      <c r="H147" s="38">
+        <v>75</v>
+      </c>
+      <c r="I147" s="39">
+        <v>76</v>
+      </c>
+      <c r="J147" s="40">
+        <v>77</v>
+      </c>
+      <c r="K147" s="42">
+        <v>78</v>
+      </c>
+      <c r="L147" s="43">
+        <v>79</v>
+      </c>
+      <c r="M147" s="44">
+        <v>80</v>
+      </c>
+      <c r="N147" s="42">
+        <v>81</v>
+      </c>
+      <c r="O147" s="43">
+        <v>82</v>
+      </c>
+      <c r="P147" s="44">
+        <v>83</v>
+      </c>
+      <c r="Q147" s="42">
+        <v>84</v>
+      </c>
+      <c r="R147" s="43">
+        <v>85</v>
+      </c>
+      <c r="S147" s="44">
+        <v>86</v>
+      </c>
+      <c r="T147" s="42">
+        <v>87</v>
+      </c>
+      <c r="U147" s="43">
+        <v>88</v>
+      </c>
+      <c r="V147" s="40">
+        <v>89</v>
+      </c>
+      <c r="W147" s="38">
+        <v>90</v>
+      </c>
+      <c r="X147" s="39">
+        <v>91</v>
+      </c>
+      <c r="Y147" s="40">
+        <v>92</v>
+      </c>
+      <c r="Z147" s="38">
+        <v>93</v>
+      </c>
+      <c r="AA147" s="39">
+        <v>94</v>
+      </c>
+      <c r="AB147" s="40">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="148" spans="3:29" x14ac:dyDescent="0.15">
+      <c r="C148">
+        <v>3</v>
+      </c>
+      <c r="E148" s="38">
+        <v>48</v>
+      </c>
+      <c r="F148" s="39">
+        <v>49</v>
+      </c>
+      <c r="G148" s="40">
+        <v>50</v>
+      </c>
+      <c r="H148" s="38">
+        <v>51</v>
+      </c>
+      <c r="I148" s="39">
+        <v>52</v>
+      </c>
+      <c r="J148" s="40">
+        <v>53</v>
+      </c>
+      <c r="K148" s="42">
+        <v>54</v>
+      </c>
+      <c r="L148" s="43">
+        <v>55</v>
+      </c>
+      <c r="M148" s="44">
+        <v>56</v>
+      </c>
+      <c r="N148" s="45">
+        <v>57</v>
+      </c>
+      <c r="O148" s="43">
+        <v>58</v>
+      </c>
+      <c r="P148" s="44">
+        <v>59</v>
+      </c>
+      <c r="Q148" s="42">
+        <v>60</v>
+      </c>
+      <c r="R148" s="43">
+        <v>61</v>
+      </c>
+      <c r="S148" s="44">
+        <v>62</v>
+      </c>
+      <c r="T148" s="42">
+        <v>63</v>
+      </c>
+      <c r="U148" s="43">
+        <v>64</v>
+      </c>
+      <c r="V148" s="40">
+        <v>65</v>
+      </c>
+      <c r="W148" s="38">
+        <v>66</v>
+      </c>
+      <c r="X148" s="39">
+        <v>67</v>
+      </c>
+      <c r="Y148" s="40">
+        <v>68</v>
+      </c>
+      <c r="Z148" s="38">
+        <v>69</v>
+      </c>
+      <c r="AA148" s="39">
+        <v>70</v>
+      </c>
+      <c r="AB148" s="40">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="149" spans="3:29" x14ac:dyDescent="0.15">
+      <c r="C149">
+        <v>2</v>
+      </c>
+      <c r="E149" s="38">
+        <v>24</v>
+      </c>
+      <c r="F149" s="39">
+        <v>25</v>
+      </c>
+      <c r="G149" s="40">
+        <v>26</v>
+      </c>
+      <c r="H149" s="38">
+        <v>27</v>
+      </c>
+      <c r="I149" s="39">
+        <v>28</v>
+      </c>
+      <c r="J149" s="40">
+        <v>29</v>
+      </c>
+      <c r="K149" s="42">
+        <v>30</v>
+      </c>
+      <c r="L149" s="43">
+        <v>31</v>
+      </c>
+      <c r="M149" s="44">
+        <v>32</v>
+      </c>
+      <c r="N149" s="42">
+        <v>33</v>
+      </c>
+      <c r="O149" s="43">
+        <v>34</v>
+      </c>
+      <c r="P149" s="44">
+        <v>35</v>
+      </c>
+      <c r="Q149" s="42">
+        <v>36</v>
+      </c>
+      <c r="R149" s="43">
+        <v>37</v>
+      </c>
+      <c r="S149" s="44">
+        <v>38</v>
+      </c>
+      <c r="T149" s="42">
+        <v>39</v>
+      </c>
+      <c r="U149" s="43">
+        <v>40</v>
+      </c>
+      <c r="V149" s="40">
+        <v>41</v>
+      </c>
+      <c r="W149" s="38">
+        <v>42</v>
+      </c>
+      <c r="X149" s="39">
+        <v>43</v>
+      </c>
+      <c r="Y149" s="40">
+        <v>44</v>
+      </c>
+      <c r="Z149" s="38">
+        <v>45</v>
+      </c>
+      <c r="AA149" s="39">
+        <v>46</v>
+      </c>
+      <c r="AB149" s="40">
+        <v>47</v>
+      </c>
+      <c r="AC149" s="35"/>
+    </row>
+    <row r="150" spans="3:29" x14ac:dyDescent="0.15">
+      <c r="C150">
+        <v>1</v>
+      </c>
+      <c r="D150" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E150" s="38">
+        <v>0</v>
+      </c>
+      <c r="F150" s="39">
+        <v>1</v>
+      </c>
+      <c r="G150" s="40">
+        <v>2</v>
+      </c>
+      <c r="H150" s="38">
+        <v>3</v>
+      </c>
+      <c r="I150" s="39">
+        <v>4</v>
+      </c>
+      <c r="J150" s="40">
+        <v>5</v>
+      </c>
+      <c r="K150" s="42">
+        <v>6</v>
+      </c>
+      <c r="L150" s="43">
+        <v>7</v>
+      </c>
+      <c r="M150" s="44">
+        <v>8</v>
+      </c>
+      <c r="N150" s="45">
+        <v>9</v>
+      </c>
+      <c r="O150" s="43">
+        <v>10</v>
+      </c>
+      <c r="P150" s="44">
+        <v>11</v>
+      </c>
+      <c r="Q150" s="42">
+        <v>12</v>
+      </c>
+      <c r="R150" s="43">
+        <v>13</v>
+      </c>
+      <c r="S150" s="44">
+        <v>14</v>
+      </c>
+      <c r="T150" s="42">
+        <v>15</v>
+      </c>
+      <c r="U150" s="43">
+        <v>16</v>
+      </c>
+      <c r="V150" s="40">
+        <v>17</v>
+      </c>
+      <c r="W150" s="38">
+        <v>18</v>
+      </c>
+      <c r="X150" s="39">
+        <v>19</v>
+      </c>
+      <c r="Y150" s="40">
+        <v>20</v>
+      </c>
+      <c r="Z150" s="38">
+        <v>21</v>
+      </c>
+      <c r="AA150" s="39">
+        <v>22</v>
+      </c>
+      <c r="AB150" s="40">
+        <v>23</v>
+      </c>
+      <c r="AC150" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <sortState ref="C143:AC150">
+    <sortCondition descending="1" ref="C143"/>
+  </sortState>
+  <mergeCells count="11">
+    <mergeCell ref="E131:L131"/>
+    <mergeCell ref="E130:L130"/>
+    <mergeCell ref="D132:D138"/>
     <mergeCell ref="D93:D120"/>
     <mergeCell ref="H92:J92"/>
     <mergeCell ref="D57:D61"/>

</xml_diff>